<commit_message>
finished the player selection, starting to work on the fight scene
</commit_message>
<xml_diff>
--- a/plot.xlsx
+++ b/plot.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="51200" windowHeight="26600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Loading" sheetId="1" r:id="rId1"/>
     <sheet name="Enter" sheetId="2" r:id="rId2"/>
     <sheet name="Player" sheetId="3" r:id="rId3"/>
+    <sheet name="Logic" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>SEGA</t>
   </si>
@@ -37,9 +38,6 @@
     <t>ERFAANISM</t>
   </si>
   <si>
-    <t>enter.jpg</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -80,13 +78,70 @@
   </si>
   <si>
     <t>27vw</t>
+  </si>
+  <si>
+    <t>enter.gif</t>
+  </si>
+  <si>
+    <t>Characters</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Skate</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>assets/images/max.jpg</t>
+  </si>
+  <si>
+    <t>assets/images/axel.jpg</t>
+  </si>
+  <si>
+    <t>assets/images/blaze.jpg</t>
+  </si>
+  <si>
+    <t>assets/images/skate.jpg</t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Stand</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Kick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +198,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -384,7 +447,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -396,25 +459,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -425,14 +473,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,50 +545,12 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -958,12 +1025,12 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1003,14 +1070,14 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1231,7 +1298,7 @@
   <dimension ref="B1:U21"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,12 +1489,12 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="J10" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1446,10 +1513,10 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -1467,12 +1534,12 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1691,223 +1758,223 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="21"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
+      <c r="E3" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
-      <c r="U3" s="23"/>
+      <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="41"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="38"/>
+      <c r="I4" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="38"/>
+      <c r="M4" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="38"/>
+      <c r="O4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="38"/>
+      <c r="S4" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="40"/>
+      <c r="U4" s="31"/>
+    </row>
+    <row r="5" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="17"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="18"/>
+    </row>
+    <row r="6" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="17"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="18"/>
+    </row>
+    <row r="7" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="33"/>
-      <c r="O4" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="47"/>
-    </row>
-    <row r="5" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="22"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="23"/>
-    </row>
-    <row r="6" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="22"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="23"/>
-    </row>
-    <row r="7" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="22"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="17"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="22"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="17"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="U7" s="29"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="43"/>
     </row>
     <row r="8" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="31"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="22"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="17"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="22"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="29"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="43"/>
     </row>
     <row r="9" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="22"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="26"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="21"/>
       <c r="T9" s="6"/>
-      <c r="U9" s="23"/>
+      <c r="U9" s="18"/>
     </row>
     <row r="10" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="22"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1915,10 +1982,10 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1926,25 +1993,25 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
-      <c r="U10" s="23"/>
+      <c r="U10" s="18"/>
     </row>
     <row r="11" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="22"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -1952,216 +2019,216 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
-      <c r="U11" s="23"/>
+      <c r="U11" s="18"/>
     </row>
     <row r="12" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="22"/>
-      <c r="C12" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="37"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="24"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="37"/>
+      <c r="I12" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="24"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="37"/>
+      <c r="L12" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="24"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="43" t="s">
-        <v>16</v>
+      <c r="O12" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="R12" s="1"/>
-      <c r="S12" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="T12" s="40"/>
-      <c r="U12" s="23"/>
+      <c r="S12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" s="27"/>
+      <c r="U12" s="18"/>
     </row>
     <row r="13" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="22"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="21"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
-      <c r="U13" s="23"/>
+      <c r="U13" s="18"/>
     </row>
     <row r="14" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="22"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="22"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="23"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="22"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
       <c r="T14" s="6"/>
-      <c r="U14" s="23"/>
+      <c r="U14" s="18"/>
     </row>
     <row r="15" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="22"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="22"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="23"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="22"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="23"/>
+      <c r="N15" s="18"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
-      <c r="U15" s="23"/>
+      <c r="U15" s="18"/>
     </row>
     <row r="16" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="22"/>
+      <c r="B16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="23"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="M16" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="N16" s="38" t="s">
-        <v>3</v>
+      <c r="J16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>2</v>
       </c>
       <c r="O16" s="6"/>
-      <c r="P16" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="U16" s="29"/>
+      <c r="P16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="U16" s="43"/>
     </row>
     <row r="17" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="22"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="23"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="22"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="23"/>
+      <c r="N17" s="18"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="23"/>
+      <c r="U17" s="18"/>
     </row>
     <row r="18" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="22"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="23"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="22"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="23"/>
+      <c r="N18" s="18"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-      <c r="U18" s="23"/>
+      <c r="U18" s="18"/>
     </row>
     <row r="19" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="22"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
-      <c r="U19" s="23"/>
+      <c r="U19" s="18"/>
     </row>
     <row r="20" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="22"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -2180,32 +2247,38 @@
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
-      <c r="U20" s="23"/>
+      <c r="U20" s="18"/>
     </row>
     <row r="21" spans="2:21" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="26"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E3:R3"/>
+    <mergeCell ref="O4:P4"/>
     <mergeCell ref="P16:S16"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="D11:G11"/>
@@ -2222,13 +2295,210 @@
     <mergeCell ref="T7:U8"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E3:R3"/>
-    <mergeCell ref="O4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.33203125" style="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="49">
+        <v>1</v>
+      </c>
+      <c r="C3" s="49">
+        <v>2</v>
+      </c>
+      <c r="D3" s="49">
+        <v>3</v>
+      </c>
+      <c r="E3" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-name.png"</f>
+        <v>assets/images/max-name.png</v>
+      </c>
+      <c r="C4" s="49" t="str">
+        <f t="shared" ref="C4:E4" si="0">"assets/images/"&amp;LOWER(C2)&amp;"-name.png"</f>
+        <v>assets/images/axel-name.png</v>
+      </c>
+      <c r="D4" s="49" t="str">
+        <f t="shared" si="0"/>
+        <v>assets/images/blaze-name.png</v>
+      </c>
+      <c r="E4" s="49" t="str">
+        <f t="shared" si="0"/>
+        <v>assets/images/skate-name.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-gold.png"</f>
+        <v>assets/images/max-gold.png</v>
+      </c>
+      <c r="C6" s="49" t="str">
+        <f t="shared" ref="C6:E6" si="1">"assets/images/"&amp;LOWER(C2)&amp;"-gold.png"</f>
+        <v>assets/images/axel-gold.png</v>
+      </c>
+      <c r="D6" s="49" t="str">
+        <f t="shared" si="1"/>
+        <v>assets/images/blaze-gold.png</v>
+      </c>
+      <c r="E6" s="49" t="str">
+        <f t="shared" si="1"/>
+        <v>assets/images/skate-gold.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-stand.gif"</f>
+        <v>assets/images/max-stand.gif</v>
+      </c>
+      <c r="C7" s="49" t="str">
+        <f t="shared" ref="C7:E7" si="2">"assets/images/"&amp;LOWER(C2)&amp;"-stand.gif"</f>
+        <v>assets/images/axel-stand.gif</v>
+      </c>
+      <c r="D7" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>assets/images/blaze-stand.gif</v>
+      </c>
+      <c r="E7" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>assets/images/skate-stand.gif</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-p1.jpg"</f>
+        <v>assets/images/max-p1.jpg</v>
+      </c>
+      <c r="C8" s="49" t="str">
+        <f t="shared" ref="C8:E8" si="3">"assets/images/"&amp;LOWER(C2)&amp;"-p1.jpg"</f>
+        <v>assets/images/axel-p1.jpg</v>
+      </c>
+      <c r="D8" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>assets/images/blaze-p1.jpg</v>
+      </c>
+      <c r="E8" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>assets/images/skate-p1.jpg</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-p2.jpg"</f>
+        <v>assets/images/max-p2.jpg</v>
+      </c>
+      <c r="C9" s="49" t="str">
+        <f t="shared" ref="C9:E9" si="4">"assets/images/"&amp;LOWER(C2)&amp;"-p2.jpg"</f>
+        <v>assets/images/axel-p2.jpg</v>
+      </c>
+      <c r="D9" s="49" t="str">
+        <f t="shared" si="4"/>
+        <v>assets/images/blaze-p2.jpg</v>
+      </c>
+      <c r="E9" s="49" t="str">
+        <f t="shared" si="4"/>
+        <v>assets/images/skate-p2.jpg</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="49" t="str">
+        <f>"assets/images/"&amp;LOWER(B2)&amp;"-kick.gif"</f>
+        <v>assets/images/max-kick.gif</v>
+      </c>
+      <c r="C10" s="49" t="str">
+        <f t="shared" ref="C10:E10" si="5">"assets/images/"&amp;LOWER(C2)&amp;"-kick.gif"</f>
+        <v>assets/images/axel-kick.gif</v>
+      </c>
+      <c r="D10" s="49" t="str">
+        <f t="shared" si="5"/>
+        <v>assets/images/blaze-kick.gif</v>
+      </c>
+      <c r="E10" s="49" t="str">
+        <f t="shared" si="5"/>
+        <v>assets/images/skate-kick.gif</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>